<commit_message>
feat: refinamiento graficos random forest final
</commit_message>
<xml_diff>
--- a/data tabla descripcion.xlsx
+++ b/data tabla descripcion.xlsx
@@ -563,7 +563,7 @@
     <col customWidth="1" min="1" max="1" width="38.86"/>
     <col customWidth="1" min="2" max="2" width="15.0"/>
     <col customWidth="1" min="3" max="3" width="10.0"/>
-    <col customWidth="1" min="4" max="4" width="27.71"/>
+    <col customWidth="1" min="4" max="4" width="27.57"/>
     <col customWidth="1" min="5" max="5" width="21.86"/>
     <col customWidth="1" min="6" max="25" width="10.71"/>
   </cols>
@@ -864,7 +864,6 @@
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
@@ -1255,7 +1254,7 @@
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24">
       <c r="A24" s="7" t="s">
         <v>63</v>
       </c>

</xml_diff>